<commit_message>
Add new kernel for bfs_rec
</commit_message>
<xml_diff>
--- a/recApps/bfs/results/results.xlsx
+++ b/recApps/bfs/results/results.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="34">
   <si>
     <t>Gitlab</t>
   </si>
@@ -107,7 +107,16 @@
     <t>http://www.cc.gatech.edu/dimacs10/archive/kronecker.shtml</t>
   </si>
   <si>
+    <t>Total storage needs (MB)</t>
+  </si>
+  <si>
     <t>No double links, no self-directed edges</t>
+  </si>
+  <si>
+    <t>Queue_Sources</t>
+  </si>
+  <si>
+    <t>too much</t>
   </si>
 </sst>
 </file>
@@ -209,10 +218,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H25"/>
+  <dimension ref="A1:O25"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E25" activeCellId="0" sqref="E25"/>
+      <selection pane="topLeft" activeCell="E10" activeCellId="0" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -390,6 +399,16 @@
       <c r="G16" s="0" t="s">
         <v>29</v>
       </c>
+      <c r="L16" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="M16" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="N16" s="0" t="n">
+        <f aca="false">B17*4/(1024*1024)</f>
+        <v>0.25</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
@@ -405,10 +424,29 @@
         <v>4912142</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F17" s="0" t="n">
         <v>20</v>
+      </c>
+      <c r="M17" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="N17" s="0" t="n">
+        <f aca="false">(D17*4)/(1024*1024)</f>
+        <v>18.7383346557617</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M18" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="N18" s="0" t="n">
+        <f aca="false">(B17*B17*4)/(1024*1024)</f>
+        <v>16384</v>
+      </c>
+      <c r="O18" s="0" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>